<commit_message>
Alteração Final de semana 10/12
</commit_message>
<xml_diff>
--- a/editaveis/preço do dia.xlsx
+++ b/editaveis/preço do dia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guilherme\Documents\Mercado Amarilho\editaveis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13260322-EC37-4C9D-B3D7-D47461FE3F95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{461F530B-B9EE-4231-8FC2-1CC9F19D7C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27480" yWindow="-120" windowWidth="27600" windowHeight="15030" xr2:uid="{2B9FEE92-7BE8-4627-BB85-CC58268006FF}"/>
+    <workbookView xWindow="-24180" yWindow="1320" windowWidth="20520" windowHeight="10785" xr2:uid="{2B9FEE92-7BE8-4627-BB85-CC58268006FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>CODIGO</t>
   </si>
@@ -40,28 +40,76 @@
     <t>C/PROMO</t>
   </si>
   <si>
-    <t>pao</t>
-  </si>
-  <si>
-    <t>queijo</t>
-  </si>
-  <si>
-    <t>presunto</t>
-  </si>
-  <si>
-    <t>mortadela</t>
-  </si>
-  <si>
-    <t>salame</t>
-  </si>
-  <si>
-    <t>leite languiru</t>
-  </si>
-  <si>
-    <t>bife</t>
-  </si>
-  <si>
-    <t>salsichao</t>
+    <t>SALSICHAO</t>
+  </si>
+  <si>
+    <t>COXA E SOBRECOXA DORSAL</t>
+  </si>
+  <si>
+    <t>PERNIL DE PORCO</t>
+  </si>
+  <si>
+    <t>CHULETA DE PORCO</t>
+  </si>
+  <si>
+    <t>PALETA DE PORCO</t>
+  </si>
+  <si>
+    <t>LINGUIÇA CALABRESA</t>
+  </si>
+  <si>
+    <t>BACON</t>
+  </si>
+  <si>
+    <t>COSTELA DE PEITO</t>
+  </si>
+  <si>
+    <t>AGULHA DE RES</t>
+  </si>
+  <si>
+    <t>COSRTE AMERICANO</t>
+  </si>
+  <si>
+    <t>BIFE DE 1</t>
+  </si>
+  <si>
+    <t>GUISADO DE 2</t>
+  </si>
+  <si>
+    <t>BATATA BRANCA</t>
+  </si>
+  <si>
+    <t>TOMATE</t>
+  </si>
+  <si>
+    <t>OVO VERMELHO</t>
+  </si>
+  <si>
+    <t>ARROZ BLUEVILLE</t>
+  </si>
+  <si>
+    <t>ERVILHA FUGINI SACHE</t>
+  </si>
+  <si>
+    <t>CAFÉ CABOCLO</t>
+  </si>
+  <si>
+    <t>SUCO EM PO POP FRUTA</t>
+  </si>
+  <si>
+    <t>CERVEJA SCHIN</t>
+  </si>
+  <si>
+    <t>REFRIGERANTE FANTA</t>
+  </si>
+  <si>
+    <t>AGUA SANITARIA 5LT</t>
+  </si>
+  <si>
+    <t>AMACIANTE GIRANDO SOL</t>
+  </si>
+  <si>
+    <t>SABAO EM PO UZZILIM</t>
   </si>
 </sst>
 </file>
@@ -97,7 +145,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -112,6 +160,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -448,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B404480-2401-45A5-917D-D1CFB61E685C}">
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,10 +517,10 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10"/>
+      <c r="C1" s="11"/>
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
@@ -479,376 +530,577 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>103</v>
-      </c>
-      <c r="B2" s="10" t="s">
+        <v>315</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="10"/>
+      <c r="C2" s="11"/>
       <c r="D2" s="2">
-        <v>6.99</v>
+        <v>12.99</v>
       </c>
       <c r="E2" s="1">
-        <v>7.99</v>
+        <v>16.989999999999998</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>121</v>
-      </c>
-      <c r="B3" s="10" t="s">
+        <v>714</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="10"/>
+      <c r="C3" s="11"/>
       <c r="D3" s="2">
-        <v>29.9</v>
+        <v>6.99</v>
       </c>
       <c r="E3" s="1">
-        <v>36.9</v>
+        <v>8.99</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>122</v>
-      </c>
-      <c r="B4" s="10" t="s">
+        <v>338</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="10"/>
+      <c r="C4" s="11"/>
       <c r="D4" s="2">
-        <v>17.899999999999999</v>
+        <v>12.99</v>
       </c>
       <c r="E4" s="8">
-        <v>20.9</v>
+        <v>14.99</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>117</v>
-      </c>
-      <c r="B5" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="10"/>
+      <c r="C5" s="11"/>
       <c r="D5" s="2">
-        <v>8.9</v>
+        <v>14.69</v>
       </c>
       <c r="E5" s="1">
-        <v>9.9</v>
+        <v>17.989999999999998</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
+      <c r="A6" s="4">
+        <v>389</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="11"/>
+      <c r="D6" s="2">
+        <v>11.99</v>
+      </c>
+      <c r="E6" s="1">
+        <v>12.99</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <v>310</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="10"/>
+        <v>301</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="11"/>
       <c r="D7" s="2">
-        <v>2.69</v>
+        <v>12.99</v>
       </c>
       <c r="E7" s="1">
-        <v>29.99</v>
+        <v>16.989999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
-        <v>7896648699453</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="2">
-        <v>3.25</v>
-      </c>
-      <c r="E8" s="1">
-        <v>3.59</v>
-      </c>
+      <c r="A8" s="9"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
-        <v>350</v>
-      </c>
-      <c r="B9" s="10" t="s">
+        <v>309</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="10"/>
+      <c r="C9" s="11"/>
       <c r="D9" s="2">
-        <v>29.99</v>
+        <v>20.99</v>
       </c>
       <c r="E9" s="1">
-        <v>34.99</v>
+        <v>26.99</v>
       </c>
       <c r="F9" s="5"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
       <c r="I9" s="4"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>315</v>
-      </c>
-      <c r="B10" s="10" t="s">
+        <v>345</v>
+      </c>
+      <c r="B10" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="10"/>
+      <c r="C10" s="11"/>
       <c r="D10" s="2">
+        <v>17.989999999999998</v>
+      </c>
+      <c r="E10" s="1">
+        <v>18.690000000000001</v>
+      </c>
+      <c r="F10" s="4"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>343</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="2">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="E11" s="1">
+        <v>20.99</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="4"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>346</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="4">
+        <v>26.99</v>
+      </c>
+      <c r="E12" s="6">
+        <v>29.99</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="4"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>350</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="4">
+        <v>29.99</v>
+      </c>
+      <c r="E13" s="4">
+        <v>34.99</v>
+      </c>
+      <c r="F13" s="4"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>361</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="4">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="E14" s="4">
+        <v>20.99</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>206</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="11"/>
+      <c r="D16" s="2">
+        <v>1.49</v>
+      </c>
+      <c r="E16" s="1">
+        <v>2.79</v>
+      </c>
+      <c r="F16" s="4"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="4"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>220</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="11"/>
+      <c r="D17" s="2">
+        <v>3.99</v>
+      </c>
+      <c r="E17" s="1">
+        <v>6.59</v>
+      </c>
+      <c r="F17" s="4"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="4"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
+        <v>267</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="11"/>
+      <c r="D18" s="2">
+        <v>10.99</v>
+      </c>
+      <c r="E18" s="1">
         <v>12.99</v>
       </c>
-      <c r="E10" s="1">
+      <c r="F18" s="4"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="4"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="10">
+        <v>7896011906874</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="11"/>
+      <c r="D19" s="2">
         <v>16.989999999999998</v>
       </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="4"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="4"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="4"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="4"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="4"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="4"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="4"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="4"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="4"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
+      <c r="E19" s="1">
+        <v>19.989999999999998</v>
+      </c>
       <c r="F19" s="4"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
       <c r="I19" s="4"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
+      <c r="A20" s="10">
+        <v>7897517209056</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="11"/>
+      <c r="D20" s="2">
+        <v>2.29</v>
+      </c>
+      <c r="E20" s="1">
+        <v>2.29</v>
+      </c>
       <c r="F20" s="4"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
       <c r="I20" s="4"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="E21" s="3"/>
+      <c r="A21" s="10">
+        <v>7896089010916</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="11"/>
+      <c r="D21" s="2">
+        <v>11.99</v>
+      </c>
+      <c r="E21" s="3">
+        <v>12.99</v>
+      </c>
       <c r="F21" s="4"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
       <c r="I21" s="4"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
       <c r="F22" s="4"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
       <c r="I22" s="4"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
+      <c r="B23" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="11"/>
+      <c r="D23" s="2">
+        <v>0.59</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0.59</v>
+      </c>
       <c r="F23" s="4"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
       <c r="I23" s="4"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
+      <c r="A24" s="10">
+        <v>7896052605316</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="11"/>
+      <c r="D24" s="2">
+        <v>2.99</v>
+      </c>
+      <c r="E24" s="1">
+        <v>3.29</v>
+      </c>
       <c r="F24" s="4"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
       <c r="I24" s="4"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
+      <c r="A25" s="10">
+        <v>7894900031515</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="11"/>
+      <c r="D25" s="2">
+        <v>6.99</v>
+      </c>
+      <c r="E25" s="1">
+        <v>6.99</v>
+      </c>
       <c r="F25" s="4"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
       <c r="I25" s="4"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
+      <c r="A26" s="10">
+        <v>7898954528038</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="11"/>
+      <c r="D26" s="2">
+        <v>6.79</v>
+      </c>
+      <c r="E26" s="1">
+        <v>7.99</v>
+      </c>
       <c r="F26" s="4"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
       <c r="I26" s="4"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
+      <c r="B27" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="11"/>
+      <c r="D27" s="2">
+        <v>3.99</v>
+      </c>
+      <c r="E27" s="1">
+        <v>4.99</v>
+      </c>
       <c r="F27" s="4"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
       <c r="I27" s="4"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
+      <c r="B28" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="11"/>
+      <c r="D28" s="2">
+        <v>6.49</v>
+      </c>
+      <c r="E28" s="1">
+        <v>6.79</v>
+      </c>
       <c r="F28" s="4"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
       <c r="I28" s="4"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
       <c r="F29" s="4"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
       <c r="I29" s="4"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
       <c r="F30" s="4"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
       <c r="I30" s="4"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
       <c r="F31" s="4"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
       <c r="I31" s="4"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
       <c r="F32" s="4"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
       <c r="I32" s="4"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
       <c r="F33" s="4"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="10"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
       <c r="I33" s="4"/>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
       <c r="F34" s="4"/>
-      <c r="G34" s="10"/>
-      <c r="H34" s="10"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
       <c r="I34" s="4"/>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
       <c r="F35" s="4"/>
-      <c r="G35" s="10"/>
-      <c r="H35" s="10"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
       <c r="I35" s="4"/>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B37" s="10"/>
-      <c r="C37" s="10"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B39" s="10"/>
-      <c r="C39" s="10"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="67">
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="B38:C38"/>
     <mergeCell ref="B39:C39"/>
     <mergeCell ref="B23:C23"/>
@@ -865,57 +1117,6 @@
     <mergeCell ref="B34:C34"/>
     <mergeCell ref="B35:C35"/>
     <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G32:H32"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>